<commit_message>
feat (member) : create clear data feature for delete all member data (foreign key problem) for add new member data
</commit_message>
<xml_diff>
--- a/public/DataAnggota/data-teater.xlsx
+++ b/public/DataAnggota/data-teater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad T480s\OneDrive - Microsoft 365\#sampah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0376AF3D-8C53-4106-9516-6E8B2D41F800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1335FB53-2FB6-4805-A324-F9E7497EFADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58C31C95-256A-41F2-8D5A-A64E5BB4A654}"/>
   </bookViews>
@@ -586,9 +586,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -624,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -644,7 +641,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DF86B6-D67A-4104-B7A5-B318497E1969}">
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,12 +970,12 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: change sidebar for admin, refactor id column, change some field on migrations
</commit_message>
<xml_diff>
--- a/public/DataAnggota/data-teater.xlsx
+++ b/public/DataAnggota/data-teater.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad T480s\OneDrive - Microsoft 365\#sampah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fazril\Kuliah\Skripsi\Dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1335FB53-2FB6-4805-A324-F9E7497EFADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD65435-1215-40C7-9023-206DC605DD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58C31C95-256A-41F2-8D5A-A64E5BB4A654}"/>
   </bookViews>
@@ -958,7 +958,7 @@
   <dimension ref="B1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor: fixing subcriteria seeder and database seeder
</commit_message>
<xml_diff>
--- a/public/DataAnggota/data-teater.xlsx
+++ b/public/DataAnggota/data-teater.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fazril\Kuliah\Skripsi\Dokumen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fazril\Kuliah\Skripsi\Dokumen\All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD65435-1215-40C7-9023-206DC605DD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D84476C-61B9-4FDE-B101-04E27ED75045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58C31C95-256A-41F2-8D5A-A64E5BB4A654}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="182">
   <si>
     <t>Anggun Damayanti</t>
   </si>
@@ -171,9 +171,6 @@
     <t>sitinursuningsih@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">JAPAR SIDIQ RAMDANI </t>
-  </si>
-  <si>
     <t>A9</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>gayuhanugrahyani@gmail.com</t>
   </si>
   <si>
-    <t>shela hutahaean</t>
-  </si>
-  <si>
     <t>A12</t>
   </si>
   <si>
@@ -402,9 +396,6 @@
     <t>elsasusila23@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">RACHELIA RACHIONADIN AFWIN NOVUTRI </t>
-  </si>
-  <si>
     <t>A25</t>
   </si>
   <si>
@@ -477,9 +468,6 @@
     <t>sitohangsarah23@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">luis pratama </t>
-  </si>
-  <si>
     <t>A30</t>
   </si>
   <si>
@@ -580,13 +568,25 @@
   </si>
   <si>
     <t>2008-01-22</t>
+  </si>
+  <si>
+    <t>Japar Sidiq Ramdani</t>
+  </si>
+  <si>
+    <t>Shela Hutahaean</t>
+  </si>
+  <si>
+    <t>Rachelia Rachionadin Afwin Novutri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis Pratama </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,13 +600,33 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -618,10 +638,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -638,14 +659,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -958,12 +997,13 @@
   <dimension ref="B1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
@@ -979,49 +1019,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="B1" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
-        <v>301280301001</v>
-      </c>
+      <c r="E1" s="4"/>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="J1" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="L1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>8</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>9</v>
+      <c r="B2" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1030,39 +1068,39 @@
         <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>18197091</v>
+        <v>14151013</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="J2" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>14</v>
+      <c r="B3" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -1071,19 +1109,19 @@
         <v>15</v>
       </c>
       <c r="E3" s="2">
-        <v>232410396</v>
+        <v>232410380</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="J3" s="1">
         <v>10</v>
@@ -1092,7 +1130,7 @@
         <v>19</v>
       </c>
       <c r="L3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>7</v>
@@ -1102,8 +1140,8 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>20</v>
+      <c r="B4" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1112,39 +1150,39 @@
         <v>21</v>
       </c>
       <c r="E4" s="2">
-        <v>232410139</v>
+        <v>19207111</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="J4" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="N4" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>25</v>
+      <c r="B5" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -1152,14 +1190,20 @@
       <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="2">
+        <v>19207128</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="I5" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="J5" s="1">
         <v>11</v>
@@ -1168,18 +1212,18 @@
         <v>6</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="N5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>28</v>
+      <c r="B6" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
@@ -1187,36 +1231,40 @@
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1">
-        <v>18197002</v>
+      <c r="E6" s="2">
+        <v>232410057</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="5"/>
+        <v>146</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="I6" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="J6" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="L6">
         <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>33</v>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
@@ -1225,39 +1273,39 @@
         <v>34</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>232410396</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="J7" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N7" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>40</v>
+      <c r="B8" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
@@ -1266,69 +1314,69 @@
         <v>41</v>
       </c>
       <c r="E8" s="2">
-        <v>12131023</v>
+        <v>19207272</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="I8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J8" s="1">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2">
+        <v>20217182</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
         <v>159</v>
       </c>
-      <c r="J8" s="1">
-        <v>12</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8">
-        <v>5</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="2">
-        <v>18197128</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" t="s">
-        <v>160</v>
-      </c>
       <c r="J9" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>7</v>
@@ -1338,37 +1386,39 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="5"/>
+        <v>137</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="I10" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="J10" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="L10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="N10" t="s">
         <v>8</v>
@@ -1376,37 +1426,37 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="E11" s="2">
-        <v>232410380</v>
+        <v>301280301001</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="J11" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>7</v>
@@ -1417,34 +1467,34 @@
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2">
-        <v>20217182</v>
+        <v>18197091</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="J12" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>2</v>
@@ -1458,30 +1508,34 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="E13" s="2">
+        <v>232410139</v>
+      </c>
       <c r="F13" s="3" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="I13" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="J13" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="L13">
         <v>4</v>
@@ -1495,28 +1549,22 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="2">
-        <v>19207111</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>70</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="J14" s="1">
         <v>11</v>
@@ -1528,80 +1576,74 @@
         <v>5</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="N14" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="2">
-        <v>19207128</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="1">
+        <v>18197002</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H15" s="5"/>
       <c r="I15" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="J15" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="N15" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="2">
-        <v>14151013</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="3" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="J16" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>38</v>
@@ -1610,77 +1652,77 @@
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="N16" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E17" s="2">
-        <v>19207272</v>
+        <v>12131023</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" t="s">
+        <v>155</v>
+      </c>
+      <c r="J17" s="1">
+        <v>12</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I17" t="s">
-        <v>168</v>
-      </c>
-      <c r="J17" s="1">
-        <v>11</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="E18" s="2">
-        <v>53134249</v>
+        <v>18197128</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="I18" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="J18" s="1">
         <v>12</v>
@@ -1689,10 +1731,10 @@
         <v>6</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="N18" t="s">
         <v>8</v>
@@ -1700,28 +1742,24 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="2">
-        <v>18197016</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="1">
-        <v>85892845822</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>98</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="5"/>
       <c r="I19" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J19" s="1">
         <v>12</v>
@@ -1730,10 +1768,10 @@
         <v>6</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="N19" t="s">
         <v>8</v>
@@ -1741,36 +1779,36 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="3" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="J20" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="N20" t="s">
         <v>8</v>
@@ -1778,40 +1816,40 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="2">
-        <v>232410383</v>
+        <v>53134249</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="I21" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="J21" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N21" t="s">
         <v>8</v>
@@ -1819,38 +1857,40 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E22" s="2">
-        <v>232410346</v>
+        <v>18197016</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H22" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="G22" s="1">
+        <v>85892845822</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="I22" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="J22" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L22">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N22" t="s">
         <v>8</v>
@@ -1858,40 +1898,36 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>114</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="H23" s="5"/>
       <c r="I23" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="J23" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="L23">
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N23" t="s">
         <v>8</v>
@@ -1899,40 +1935,40 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E24" s="2">
-        <v>18197086</v>
+        <v>232410383</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="I24" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="J24" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="L24">
         <v>1</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N24" t="s">
         <v>8</v>
@@ -1940,26 +1976,26 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="4"/>
+        <v>120</v>
+      </c>
+      <c r="E25" s="2">
+        <v>232410346</v>
+      </c>
       <c r="F25" s="3" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>126</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="H25" s="5"/>
       <c r="I25" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="J25" s="1">
         <v>10</v>
@@ -1968,10 +2004,10 @@
         <v>19</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N25" t="s">
         <v>8</v>
@@ -1979,36 +2015,40 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="E26" s="6">
+        <v>67169146</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="G26" s="3" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="I26" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="J26" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L26">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N26" t="s">
         <v>8</v>
@@ -2016,77 +2056,79 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E27" s="4"/>
+        <v>129</v>
+      </c>
+      <c r="E27" s="2">
+        <v>18197086</v>
+      </c>
       <c r="F27" s="3" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" t="s">
+        <v>171</v>
+      </c>
+      <c r="J27" s="1">
+        <v>12</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="I27" t="s">
-        <v>178</v>
-      </c>
-      <c r="J27" s="1">
-        <v>10</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="3" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="I28" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="J28" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="L28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N28" t="s">
         <v>8</v>
@@ -2094,28 +2136,24 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" s="2">
-        <v>201280301025</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>144</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="3" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="I29" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J29" s="1">
         <v>10</v>
@@ -2124,39 +2162,39 @@
         <v>19</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N29" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E30" s="2">
-        <v>232410057</v>
+        <v>201280301025</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="I30" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="J30" s="1">
         <v>10</v>
@@ -2165,17 +2203,24 @@
         <v>19</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N30" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B30">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H21" r:id="rId1" xr:uid="{CF8B0A05-B71A-4151-8C62-BEF2BCB9462C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated: featured updated (fix-sidang)
</commit_message>
<xml_diff>
--- a/public/DataAnggota/data-teater.xlsx
+++ b/public/DataAnggota/data-teater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fazril\Kuliah\Skripsi\Dokumen\All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D84476C-61B9-4FDE-B101-04E27ED75045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A779BF-705F-46C1-BECF-A378283985FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58C31C95-256A-41F2-8D5A-A64E5BB4A654}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="183">
   <si>
     <t>Anggun Damayanti</t>
   </si>
@@ -580,6 +580,9 @@
   </si>
   <si>
     <t xml:space="preserve">Luis Pratama </t>
+  </si>
+  <si>
+    <t>qw3esdwxsergfdsx</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1000,7 @@
   <dimension ref="B1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1765,7 +1768,7 @@
         <v>12</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>6</v>
+        <v>182</v>
       </c>
       <c r="L19">
         <v>3</v>

</xml_diff>